<commit_message>
Updated code to log score
</commit_message>
<xml_diff>
--- a/bin/.xlsx/component_3.xlsx
+++ b/bin/.xlsx/component_3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Nextcloud\code\behavior_contrast_main_v1.0.3\bin\.xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gseagles-my.sharepoint.com/personal/mw24396_georgiasouthern_edu/Documents/4_RESEARCH/behavior_contrast/behavioral_contrast_psychopy/bin/.xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8119ED77-8E98-4DF6-BAAA-C1B380FF5925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{8119ED77-8E98-4DF6-BAAA-C1B380FF5925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECE5E551-3CE7-4C23-A1ED-222B41DAA745}"/>
   <bookViews>
-    <workbookView xWindow="11970" yWindow="1680" windowWidth="15570" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7875" yWindow="1920" windowWidth="13500" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -712,7 +712,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -751,10 +751,10 @@
     </row>
     <row r="2" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>120</v>
@@ -1109,18 +1109,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1140,6 +1140,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1152,12 +1160,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>